<commit_message>
PathPlanningUsingMpc: change states to x y theta v alpha, and inputs to a w
</commit_message>
<xml_diff>
--- a/PathPlanningUsingMpc/规划结果/README.xlsx
+++ b/PathPlanningUsingMpc/规划结果/README.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\PathPlanningUsingMpc\规划结果\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA44ED3B-E809-4F21-9632-F0CF379990B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E49DD70-44BD-4890-915F-FC52B33DC0A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1470" windowWidth="14400" windowHeight="8723" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
-  <si>
-    <t>obs5-10-22-35</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>p</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -48,33 +45,23 @@
     <t>targetPose</t>
   </si>
   <si>
-    <t>[-4.5;0;0]</t>
-  </si>
-  <si>
-    <t>[4.5;0;0]</t>
-  </si>
-  <si>
     <t>cost</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>diag([0.1 0.1 0.1])</t>
+    <t>obs05-15-10-42</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>obs5-10-23-09</t>
+    <t>[-4.5;0;0]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve"> 1*eye(2)</t>
+    <t>[4.5;0;0]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>obs5-11-10-11</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3*eye(2)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>diag([0 0 0 0.1 0.1])</t>
   </si>
 </sst>
 </file>
@@ -420,48 +407,48 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.06640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.46484375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.46484375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.625" customWidth="1"/>
+    <col min="2" max="2" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.875" customWidth="1"/>
+    <col min="7" max="7" width="8.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="G1" s="4"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="D2" s="2">
         <v>200</v>
@@ -469,60 +456,32 @@
       <c r="E2" s="3">
         <v>0.05</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="2">
-        <v>200</v>
-      </c>
-      <c r="E3" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="2">
-        <v>200</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -531,7 +490,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -540,7 +499,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -549,7 +508,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -558,7 +517,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -567,7 +526,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -576,7 +535,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -585,7 +544,7 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -594,7 +553,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -603,7 +562,7 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -612,7 +571,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -621,7 +580,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -630,7 +589,7 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -639,7 +598,7 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -648,7 +607,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -657,7 +616,7 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -666,7 +625,7 @@
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -675,7 +634,7 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -684,7 +643,7 @@
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -693,7 +652,7 @@
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -702,7 +661,7 @@
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -711,7 +670,7 @@
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -720,7 +679,7 @@
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -729,7 +688,7 @@
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -738,7 +697,7 @@
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -747,7 +706,7 @@
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>

</xml_diff>